<commit_message>
Added "LiteralFSA" which is used to identify strings that appear like: 'I'm a string' or Run_Strings which never close and are errors.
</commit_message>
<xml_diff>
--- a/MicroPascalCompiler/uPascal_Tokens_List.xlsx
+++ b/MicroPascalCompiler/uPascal_Tokens_List.xlsx
@@ -599,15 +599,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -698,8 +698,8 @@
   </sheetPr>
   <dimension ref="A1:B76"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A48" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A76" activeCellId="1" sqref="A73:A74 A76"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A51" activeCellId="0" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1054,7 +1054,7 @@
       </c>
     </row>
     <row r="49" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="13" t="s">
+      <c r="A49" s="7" t="s">
         <v>82</v>
       </c>
       <c r="B49" s="9" t="s">
@@ -1062,13 +1062,13 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="14" t="s">
+      <c r="A51" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="B51" s="14"/>
+      <c r="B51" s="13"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="15" t="s">
+      <c r="A53" s="14" t="s">
         <v>85</v>
       </c>
       <c r="B53" s="8" t="s">
@@ -1076,7 +1076,7 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="15" t="s">
+      <c r="A54" s="14" t="s">
         <v>87</v>
       </c>
       <c r="B54" s="8" t="s">
@@ -1084,7 +1084,7 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="15" t="s">
+      <c r="A55" s="14" t="s">
         <v>89</v>
       </c>
       <c r="B55" s="8" t="s">
@@ -1092,7 +1092,7 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="15" t="s">
+      <c r="A56" s="14" t="s">
         <v>91</v>
       </c>
       <c r="B56" s="8" t="s">
@@ -1100,7 +1100,7 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="13" t="s">
+      <c r="A57" s="15" t="s">
         <v>93</v>
       </c>
       <c r="B57" s="9" t="s">
@@ -1108,7 +1108,7 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="15" t="s">
+      <c r="A58" s="14" t="s">
         <v>95</v>
       </c>
       <c r="B58" s="8" t="s">
@@ -1116,7 +1116,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="15" t="s">
+      <c r="A59" s="14" t="s">
         <v>97</v>
       </c>
       <c r="B59" s="8" t="s">
@@ -1124,7 +1124,7 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="15" t="s">
+      <c r="A60" s="14" t="s">
         <v>99</v>
       </c>
       <c r="B60" s="8" t="s">
@@ -1132,7 +1132,7 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="15" t="s">
+      <c r="A61" s="14" t="s">
         <v>101</v>
       </c>
       <c r="B61" s="8" t="s">
@@ -1140,7 +1140,7 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="15" t="s">
+      <c r="A62" s="14" t="s">
         <v>103</v>
       </c>
       <c r="B62" s="8" t="s">
@@ -1148,7 +1148,7 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="15" t="s">
+      <c r="A63" s="14" t="s">
         <v>105</v>
       </c>
       <c r="B63" s="8" t="s">
@@ -1156,7 +1156,7 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="15" t="s">
+      <c r="A64" s="14" t="s">
         <v>107</v>
       </c>
       <c r="B64" s="8" t="s">
@@ -1164,7 +1164,7 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="15" t="s">
+      <c r="A65" s="14" t="s">
         <v>109</v>
       </c>
       <c r="B65" s="8" t="s">
@@ -1172,7 +1172,7 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="15" t="s">
+      <c r="A66" s="14" t="s">
         <v>111</v>
       </c>
       <c r="B66" s="8" t="s">
@@ -1180,7 +1180,7 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="15" t="s">
+      <c r="A67" s="14" t="s">
         <v>113</v>
       </c>
       <c r="B67" s="8" t="s">
@@ -1188,7 +1188,7 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="15" t="s">
+      <c r="A68" s="14" t="s">
         <v>115</v>
       </c>
       <c r="B68" s="8" t="s">
@@ -1204,10 +1204,10 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="14" t="s">
+      <c r="A71" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="B71" s="14"/>
+      <c r="B71" s="13"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="7" t="s">
@@ -1226,7 +1226,7 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="15" t="s">
+      <c r="A75" s="7" t="s">
         <v>124</v>
       </c>
       <c r="B75" s="8" t="s">

</xml_diff>

<commit_message>
Completed last of FSA's.  All token's now accounted for.
Added Symbol check to Characters class.

Added case for symbols in Dispatcher.

Completed SymbolFSA state machine.

Updated token list to reflect completion.

Added a missing type to TokenType enum.
</commit_message>
<xml_diff>
--- a/MicroPascalCompiler/uPascal_Tokens_List.xlsx
+++ b/MicroPascalCompiler/uPascal_Tokens_List.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="463" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -546,7 +546,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -601,18 +601,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -698,8 +686,8 @@
   </sheetPr>
   <dimension ref="A1:B76"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A51" activeCellId="0" sqref="A51"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A51" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A53" activeCellId="0" sqref="A53:A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1068,7 +1056,7 @@
       <c r="B51" s="13"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="14" t="s">
+      <c r="A53" s="7" t="s">
         <v>85</v>
       </c>
       <c r="B53" s="8" t="s">
@@ -1076,7 +1064,7 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="14" t="s">
+      <c r="A54" s="7" t="s">
         <v>87</v>
       </c>
       <c r="B54" s="8" t="s">
@@ -1084,7 +1072,7 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="14" t="s">
+      <c r="A55" s="7" t="s">
         <v>89</v>
       </c>
       <c r="B55" s="8" t="s">
@@ -1092,7 +1080,7 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="14" t="s">
+      <c r="A56" s="7" t="s">
         <v>91</v>
       </c>
       <c r="B56" s="8" t="s">
@@ -1100,7 +1088,7 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="15" t="s">
+      <c r="A57" s="7" t="s">
         <v>93</v>
       </c>
       <c r="B57" s="9" t="s">
@@ -1108,7 +1096,7 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="14" t="s">
+      <c r="A58" s="7" t="s">
         <v>95</v>
       </c>
       <c r="B58" s="8" t="s">
@@ -1116,7 +1104,7 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="14" t="s">
+      <c r="A59" s="7" t="s">
         <v>97</v>
       </c>
       <c r="B59" s="8" t="s">
@@ -1124,7 +1112,7 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="14" t="s">
+      <c r="A60" s="7" t="s">
         <v>99</v>
       </c>
       <c r="B60" s="8" t="s">
@@ -1132,7 +1120,7 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="14" t="s">
+      <c r="A61" s="7" t="s">
         <v>101</v>
       </c>
       <c r="B61" s="8" t="s">
@@ -1140,7 +1128,7 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="14" t="s">
+      <c r="A62" s="7" t="s">
         <v>103</v>
       </c>
       <c r="B62" s="8" t="s">
@@ -1148,7 +1136,7 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="14" t="s">
+      <c r="A63" s="7" t="s">
         <v>105</v>
       </c>
       <c r="B63" s="8" t="s">
@@ -1156,7 +1144,7 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="14" t="s">
+      <c r="A64" s="7" t="s">
         <v>107</v>
       </c>
       <c r="B64" s="8" t="s">
@@ -1164,7 +1152,7 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="14" t="s">
+      <c r="A65" s="7" t="s">
         <v>109</v>
       </c>
       <c r="B65" s="8" t="s">
@@ -1172,7 +1160,7 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="14" t="s">
+      <c r="A66" s="7" t="s">
         <v>111</v>
       </c>
       <c r="B66" s="8" t="s">
@@ -1180,7 +1168,7 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="14" t="s">
+      <c r="A67" s="7" t="s">
         <v>113</v>
       </c>
       <c r="B67" s="8" t="s">
@@ -1188,7 +1176,7 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="14" t="s">
+      <c r="A68" s="7" t="s">
         <v>115</v>
       </c>
       <c r="B68" s="8" t="s">
@@ -1196,10 +1184,10 @@
       </c>
     </row>
     <row r="69" s="10" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="16" t="s">
+      <c r="A69" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="B69" s="17" t="s">
+      <c r="B69" s="14" t="s">
         <v>118</v>
       </c>
     </row>

</xml_diff>